<commit_message>
updated functions for monte carlo, added assessment factor soil to change with assessment factor groundwater
</commit_message>
<xml_diff>
--- a/research/Monte_carlo/output/mean_1%.xlsx
+++ b/research/Monte_carlo/output/mean_1%.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>pipe_length</t>
+          <t>length_pipe</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3.988215606793845e-07</v>
+        <v>6.191157879075536e-07</v>
       </c>
       <c r="C2" t="n">
         <v>0.006120181389845239</v>
@@ -567,7 +567,7 @@
         <v>-12.24429479261075</v>
       </c>
       <c r="G2" t="n">
-        <v>2.234360796388206</v>
+        <v>3.468721592776412</v>
       </c>
       <c r="H2" t="n">
         <v>6.90979573</v>
@@ -579,7 +579,7 @@
         <v>3.468721592776412</v>
       </c>
       <c r="K2" t="n">
-        <v>0.01960000038</v>
+        <v>0.0196</v>
       </c>
       <c r="L2" t="n">
         <v>0.25</v>
@@ -621,11 +621,11 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>pipe_length</t>
+          <t>length_pipe</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.948728161935644e-07</v>
+        <v>6.129859035316447e-07</v>
       </c>
       <c r="C3" t="n">
         <v>0.006059585534500237</v>
@@ -640,7 +640,7 @@
         <v>-12.2442948083055</v>
       </c>
       <c r="G3" t="n">
-        <v>2.234360796388206</v>
+        <v>3.468721592776412</v>
       </c>
       <c r="H3" t="n">
         <v>6.9788936873</v>
@@ -652,7 +652,7 @@
         <v>3.468721592776412</v>
       </c>
       <c r="K3" t="n">
-        <v>0.01960000038</v>
+        <v>0.0196</v>
       </c>
       <c r="L3" t="n">
         <v>0.25</v>
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3.957564532875195e-07</v>
+        <v>6.129859035316447e-07</v>
       </c>
       <c r="C4" t="n">
         <v>0.006059585534500237</v>
@@ -713,7 +713,7 @@
         <v>-12.2442948083055</v>
       </c>
       <c r="G4" t="n">
-        <v>2.239360796388206</v>
+        <v>3.468721592776412</v>
       </c>
       <c r="H4" t="n">
         <v>6.90979573</v>
@@ -725,7 +725,7 @@
         <v>3.468721592776412</v>
       </c>
       <c r="K4" t="n">
-        <v>0.01960000038</v>
+        <v>0.0196</v>
       </c>
       <c r="L4" t="n">
         <v>0.25</v>
@@ -771,7 +771,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.979379072615448e-07</v>
+        <v>6.191146263107422e-07</v>
       </c>
       <c r="C5" t="n">
         <v>0.006059585534500237</v>
@@ -786,7 +786,7 @@
         <v>-12.2442948083055</v>
       </c>
       <c r="G5" t="n">
-        <v>2.251704404352088</v>
+        <v>3.503408808704176</v>
       </c>
       <c r="H5" t="n">
         <v>6.90979573</v>
@@ -798,7 +798,7 @@
         <v>3.503408808704176</v>
       </c>
       <c r="K5" t="n">
-        <v>0.01960000038</v>
+        <v>0.0196</v>
       </c>
       <c r="L5" t="n">
         <v>0.25</v>
@@ -844,7 +844,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.988215443554999e-07</v>
+        <v>6.191146263107422e-07</v>
       </c>
       <c r="C6" t="n">
         <v>0.006059585534500237</v>
@@ -859,7 +859,7 @@
         <v>-12.2442948083055</v>
       </c>
       <c r="G6" t="n">
-        <v>2.234360796388206</v>
+        <v>3.468721592776412</v>
       </c>
       <c r="H6" t="n">
         <v>6.90979573</v>
@@ -871,7 +871,7 @@
         <v>3.468721592776412</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0197960003838</v>
+        <v>0.019796</v>
       </c>
       <c r="L6" t="n">
         <v>0.25</v>
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.909638474452908e-07</v>
+        <v>6.069167361699452e-07</v>
       </c>
       <c r="C7" t="n">
         <v>0.006059585534500237</v>
@@ -932,7 +932,7 @@
         <v>-12.2442948083055</v>
       </c>
       <c r="G7" t="n">
-        <v>2.234360796388206</v>
+        <v>3.468721592776412</v>
       </c>
       <c r="H7" t="n">
         <v>6.90979573</v>
@@ -944,7 +944,7 @@
         <v>3.468721592776412</v>
       </c>
       <c r="K7" t="n">
-        <v>0.01960000038</v>
+        <v>0.0196</v>
       </c>
       <c r="L7" t="n">
         <v>0.2525</v>
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3.988215443554988e-07</v>
+        <v>6.191146263107405e-07</v>
       </c>
       <c r="C8" t="n">
         <v>0.006059585534500237</v>
@@ -1005,7 +1005,7 @@
         <v>-12.23997343452286</v>
       </c>
       <c r="G8" t="n">
-        <v>2.234360796388206</v>
+        <v>3.468721592776412</v>
       </c>
       <c r="H8" t="n">
         <v>6.90979573</v>
@@ -1017,7 +1017,7 @@
         <v>3.468721592776412</v>
       </c>
       <c r="K8" t="n">
-        <v>0.01960000038</v>
+        <v>0.0196</v>
       </c>
       <c r="L8" t="n">
         <v>0.25</v>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3.988215443555001e-07</v>
+        <v>6.191146263107423e-07</v>
       </c>
       <c r="C9" t="n">
         <v>0.006059585534500237</v>
@@ -1078,7 +1078,7 @@
         <v>-12.2442948083055</v>
       </c>
       <c r="G9" t="n">
-        <v>2.234360796388206</v>
+        <v>3.468721592776412</v>
       </c>
       <c r="H9" t="n">
         <v>6.90979573</v>
@@ -1090,7 +1090,7 @@
         <v>3.468721592776412</v>
       </c>
       <c r="K9" t="n">
-        <v>0.01960000038</v>
+        <v>0.0196</v>
       </c>
       <c r="L9" t="n">
         <v>0.25</v>
@@ -1136,7 +1136,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3.913250084826244e-07</v>
+        <v>6.074773882083438e-07</v>
       </c>
       <c r="C10" t="n">
         <v>0.006059585534500237</v>
@@ -1151,7 +1151,7 @@
         <v>-12.24821517865943</v>
       </c>
       <c r="G10" t="n">
-        <v>2.234360796388206</v>
+        <v>3.468721592776412</v>
       </c>
       <c r="H10" t="n">
         <v>6.90979573</v>
@@ -1163,7 +1163,7 @@
         <v>3.468721592776412</v>
       </c>
       <c r="K10" t="n">
-        <v>0.01960000038</v>
+        <v>0.0196</v>
       </c>
       <c r="L10" t="n">
         <v>0.25</v>
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3.939287782617742e-07</v>
+        <v>6.115202449093061e-07</v>
       </c>
       <c r="C11" t="n">
         <v>0.006059585534500237</v>
@@ -1224,7 +1224,7 @@
         <v>-12.2442948083055</v>
       </c>
       <c r="G11" t="n">
-        <v>2.234360796388206</v>
+        <v>3.468721592776412</v>
       </c>
       <c r="H11" t="n">
         <v>6.90979573</v>
@@ -1236,7 +1236,7 @@
         <v>3.468721592776412</v>
       </c>
       <c r="K11" t="n">
-        <v>0.01960000038</v>
+        <v>0.0196</v>
       </c>
       <c r="L11" t="n">
         <v>0.25</v>
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3.921092876355396e-07</v>
+        <v>6.086948719906519e-07</v>
       </c>
       <c r="C12" t="n">
         <v>0.006059585534500237</v>
@@ -1297,7 +1297,7 @@
         <v>-12.24734565271743</v>
       </c>
       <c r="G12" t="n">
-        <v>2.234360796388206</v>
+        <v>3.468721592776412</v>
       </c>
       <c r="H12" t="n">
         <v>6.90979573</v>
@@ -1309,7 +1309,7 @@
         <v>3.468721592776412</v>
       </c>
       <c r="K12" t="n">
-        <v>0.01960000038</v>
+        <v>0.0196</v>
       </c>
       <c r="L12" t="n">
         <v>0.25</v>
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3.942231986351047e-07</v>
+        <v>6.11977461345472e-07</v>
       </c>
       <c r="C13" t="n">
         <v>0.006059585534500237</v>
@@ -1370,7 +1370,7 @@
         <v>-12.2442948083055</v>
       </c>
       <c r="G13" t="n">
-        <v>2.234360796388206</v>
+        <v>3.468721592776412</v>
       </c>
       <c r="H13" t="n">
         <v>6.90979573</v>
@@ -1382,7 +1382,7 @@
         <v>3.468721592776412</v>
       </c>
       <c r="K13" t="n">
-        <v>0.01960000038</v>
+        <v>0.0196</v>
       </c>
       <c r="L13" t="n">
         <v>0.25</v>

</xml_diff>